<commit_message>
Data loading of base data successful, small tweaks to db schema
</commit_message>
<xml_diff>
--- a/python/data_builder.xlsx
+++ b/python/data_builder.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="ingredients" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="step_types" sheetId="2" r:id="rId2"/>
+    <sheet name="steps" sheetId="3" r:id="rId3"/>
+    <sheet name="units" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
@@ -24,9 +25,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -64,6 +62,63 @@
   </si>
   <si>
     <t>white granulated</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>step_type_id</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Boil</t>
+  </si>
+  <si>
+    <t>Let boil</t>
+  </si>
+  <si>
+    <t>Let simmer</t>
+  </si>
+  <si>
+    <t>Let cook</t>
+  </si>
+  <si>
+    <t>Bring to a boil</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>serving</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>unit_id</t>
+  </si>
+  <si>
+    <t>cup</t>
+  </si>
+  <si>
+    <t>onion</t>
+  </si>
+  <si>
+    <t>medium white</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -405,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,21 +480,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
         <v>0.59299999999999997</v>
@@ -447,10 +502,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>0.83</v>
@@ -458,10 +513,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="1">
         <v>2.17</v>
@@ -469,7 +524,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -477,10 +532,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="1">
         <v>0.81</v>
@@ -488,13 +543,30 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
       <c r="E7" s="1">
         <v>1.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>225</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -504,24 +576,154 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data for recipe and recipe_steps
</commit_message>
<xml_diff>
--- a/python/data_builder.xlsx
+++ b/python/data_builder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="5"/>
+    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="2"/>
     <workbookView xWindow="180" yWindow="105" windowWidth="13560" windowHeight="13110" activeTab="5"/>
   </bookViews>
   <sheets>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -61,27 +61,9 @@
     <t>step_type_id</t>
   </si>
   <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>Boil</t>
-  </si>
-  <si>
-    <t>Let boil</t>
-  </si>
-  <si>
-    <t>Let simmer</t>
-  </si>
-  <si>
-    <t>Let cook</t>
-  </si>
-  <si>
     <t>Bring to a boil</t>
   </si>
   <si>
-    <t>Mix</t>
-  </si>
-  <si>
     <t>serving</t>
   </si>
   <si>
@@ -152,6 +134,36 @@
   </si>
   <si>
     <t>white basmati rice</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>let boil</t>
+  </si>
+  <si>
+    <t>let simmer</t>
+  </si>
+  <si>
+    <t>let cook</t>
+  </si>
+  <si>
+    <t>boil</t>
+  </si>
+  <si>
+    <t>mix</t>
+  </si>
+  <si>
+    <t>rinse</t>
+  </si>
+  <si>
+    <t>fluff</t>
+  </si>
+  <si>
+    <t>serve</t>
+  </si>
+  <si>
+    <t>Fluff with fork</t>
   </si>
 </sst>
 </file>
@@ -496,7 +508,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -511,10 +523,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -525,7 +537,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -536,7 +548,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -547,7 +559,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -558,7 +570,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -577,7 +589,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -588,7 +600,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -599,13 +611,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D9">
         <v>225</v>
@@ -623,9 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,17 +650,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -660,10 +670,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -686,53 +696,80 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -758,17 +795,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +818,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -796,7 +833,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -805,10 +842,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -816,10 +853,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -833,10 +870,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -855,13 +892,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,21 +910,209 @@
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
         <v>2</v>
+      </c>
+      <c r="F10">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
converting to importing excel directly
</commit_message>
<xml_diff>
--- a/python/data_builder.xlsx
+++ b/python/data_builder.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="2"/>
+    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="4"/>
     <workbookView xWindow="180" yWindow="105" windowWidth="13560" windowHeight="13110" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="ingredients" sheetId="1" r:id="rId1"/>
-    <sheet name="step_types" sheetId="2" r:id="rId2"/>
-    <sheet name="steps" sheetId="3" r:id="rId3"/>
-    <sheet name="units" sheetId="4" r:id="rId4"/>
+    <sheet name="units" sheetId="4" r:id="rId1"/>
+    <sheet name="ingredients" sheetId="1" r:id="rId2"/>
+    <sheet name="step_types" sheetId="2" r:id="rId3"/>
+    <sheet name="steps" sheetId="3" r:id="rId4"/>
     <sheet name="recipes" sheetId="5" r:id="rId5"/>
     <sheet name="recipe_steps" sheetId="6" r:id="rId6"/>
   </sheets>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -136,9 +136,6 @@
     <t>white basmati rice</t>
   </si>
   <si>
-    <t>order</t>
-  </si>
-  <si>
     <t>let boil</t>
   </si>
   <si>
@@ -164,13 +161,19 @@
   </si>
   <si>
     <t>Fluff with fork</t>
+  </si>
+  <si>
+    <t>let rest</t>
+  </si>
+  <si>
+    <t>Allow to rest off heat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,16 +181,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -195,15 +230,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,12 +562,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6"/>
+  </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -631,7 +731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -668,18 +768,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -704,7 +810,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -712,7 +818,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -720,7 +826,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -728,7 +834,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -739,7 +845,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -747,7 +853,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -755,10 +861,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -766,46 +872,21 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -815,12 +896,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -892,230 +978,218 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14" style="6" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D6" s="3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E11" s="3">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E12" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>ingredients!$A$2:$A$100</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>recipes!$B:$B</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All db values now parsed from excel, except for recipe_steps
</commit_message>
<xml_diff>
--- a/python/data_builder.xlsx
+++ b/python/data_builder.xlsx
@@ -4,8 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="4"/>
-    <workbookView xWindow="180" yWindow="105" windowWidth="13560" windowHeight="13110" activeTab="5"/>
+    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="4" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -112,9 +111,6 @@
     <t>basmati rice</t>
   </si>
   <si>
-    <t>all purpose flower</t>
-  </si>
-  <si>
     <t>table salt</t>
   </si>
   <si>
@@ -167,6 +163,21 @@
   </si>
   <si>
     <t>Allow to rest off heat</t>
+  </si>
+  <si>
+    <t>all purpose flour</t>
+  </si>
+  <si>
+    <t>derp ingredient</t>
+  </si>
+  <si>
+    <t>derp</t>
+  </si>
+  <si>
+    <t>million</t>
+  </si>
+  <si>
+    <t>unit_weight</t>
   </si>
 </sst>
 </file>
@@ -565,10 +576,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,13 +611,10 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,13 +628,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -637,7 +642,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -659,7 +664,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -670,7 +675,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -689,7 +694,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -700,7 +705,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -711,7 +716,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -724,6 +729,17 @@
       </c>
       <c r="E9" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +752,6 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -775,11 +790,8 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +822,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -818,7 +830,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -826,7 +838,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -834,7 +846,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -845,7 +857,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -853,7 +865,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -861,10 +873,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -872,7 +884,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -880,10 +892,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -901,11 +913,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +951,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -959,7 +968,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -982,9 +991,6 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1021,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>19</v>
@@ -1029,7 +1035,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>19</v>
@@ -1043,13 +1049,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
@@ -1057,18 +1063,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="D6" s="3">
         <v>1200</v>
@@ -1076,10 +1082,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3">
         <v>300</v>
@@ -1087,29 +1093,29 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="3">
         <v>190</v>
@@ -1117,7 +1123,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>19</v>
@@ -1131,13 +1137,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3">
         <v>5.5</v>
@@ -1145,10 +1151,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3">
         <v>2700</v>
@@ -1156,18 +1162,18 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished writing to db. Significant simplification to database, read steps from db
</commit_message>
<xml_diff>
--- a/python/data_builder.xlsx
+++ b/python/data_builder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="3"/>
+    <workbookView xWindow="13890" yWindow="75" windowWidth="13455" windowHeight="13185" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <t>name</t>
   </si>
@@ -96,15 +96,9 @@
     <t>servings</t>
   </si>
   <si>
-    <t>ingredient_id</t>
-  </si>
-  <si>
     <t>recipe_id</t>
   </si>
   <si>
-    <t>step_id</t>
-  </si>
-  <si>
     <t>seconds</t>
   </si>
   <si>
@@ -178,6 +172,18 @@
   </si>
   <si>
     <t>unit_weight</t>
+  </si>
+  <si>
+    <t>ingredient</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>White basmati rice</t>
+  </si>
+  <si>
+    <t>Long grain brown rice</t>
   </si>
 </sst>
 </file>
@@ -614,7 +620,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,13 +634,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -642,7 +648,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -653,7 +659,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -664,7 +670,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -675,7 +681,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -694,7 +700,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -705,7 +711,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -716,7 +722,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -733,13 +739,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
         <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -790,8 +796,8 @@
   </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +828,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -830,7 +836,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -838,7 +844,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
@@ -846,7 +852,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -857,7 +863,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -865,7 +871,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -873,10 +879,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -884,7 +890,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -892,10 +898,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -913,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +957,7 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
@@ -968,7 +974,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -990,7 +996,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,16 +1010,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1021,13 +1027,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -1035,7 +1041,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>19</v>
@@ -1049,13 +1055,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3">
         <v>3</v>
@@ -1063,18 +1069,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="3">
         <v>1200</v>
@@ -1082,10 +1088,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3">
         <v>300</v>
@@ -1093,29 +1099,29 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3">
         <v>190</v>
@@ -1123,7 +1129,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>19</v>
@@ -1137,13 +1143,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12" s="3">
         <v>5.5</v>
@@ -1151,10 +1157,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="3">
         <v>2700</v>
@@ -1162,18 +1168,18 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1181,13 +1187,7 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>ingredients!$A$2:$A$100</xm:f>
-          </x14:formula1>
-          <xm:sqref>C1:C1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>recipes!$B:$B</xm:f>

</xml_diff>